<commit_message>
Update mark for HaiTCT
</commit_message>
<xml_diff>
--- a/Document/Report/ReportMark.xlsx
+++ b/Document/Report/ReportMark.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>Document</t>
   </si>
@@ -67,13 +67,25 @@
   </si>
   <si>
     <t>Reriew carefully</t>
+  </si>
+  <si>
+    <t>Report 01 (Review + modify)</t>
+  </si>
+  <si>
+    <t>Report 04 ( Page 42-46, 56-74)</t>
+  </si>
+  <si>
+    <t>Report 03 SRS_PMS (Page 19-32, 39-64), User Requirement_PMS(4.Project Eye, 7.Admin)</t>
+  </si>
+  <si>
+    <t>Finish task on time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -243,12 +255,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,12 +267,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -345,6 +365,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -379,6 +400,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -554,15 +576,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.5703125" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" customWidth="1"/>
@@ -575,26 +597,26 @@
     <col min="10" max="18" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="12" customFormat="1" ht="23.25">
+    <row r="1" spans="1:18" s="12" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="21"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
@@ -605,7 +627,7 @@
       <c r="Q1" s="11"/>
       <c r="R1" s="11"/>
     </row>
-    <row r="2" spans="1:18" s="16" customFormat="1">
+    <row r="2" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="14" t="s">
         <v>1</v>
@@ -641,26 +663,26 @@
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="22"/>
+      <c r="H3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="18"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -673,7 +695,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -686,7 +708,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -699,7 +721,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -712,7 +734,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -723,7 +745,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -734,7 +756,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -745,7 +767,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -756,7 +778,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -767,7 +789,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -778,7 +800,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -789,7 +811,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -800,7 +822,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1">
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -811,24 +833,24 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:18" s="4" customFormat="1">
+    <row r="17" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19" t="s">
+      <c r="E17" s="18"/>
+      <c r="F17" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="19" t="s">
+      <c r="G17" s="18"/>
+      <c r="H17" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="20"/>
+      <c r="I17" s="18"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -839,7 +861,7 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
     </row>
-    <row r="18" spans="1:18" s="4" customFormat="1">
+    <row r="18" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -861,7 +883,7 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
     </row>
-    <row r="19" spans="1:18" s="4" customFormat="1">
+    <row r="19" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -883,7 +905,7 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="20" spans="1:18" s="4" customFormat="1">
+    <row r="20" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -905,7 +927,7 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
     </row>
-    <row r="21" spans="1:18" s="4" customFormat="1">
+    <row r="21" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -927,7 +949,7 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="1:18" s="4" customFormat="1">
+    <row r="22" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -947,7 +969,7 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
     </row>
-    <row r="23" spans="1:18" s="4" customFormat="1">
+    <row r="23" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -967,7 +989,7 @@
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
     </row>
-    <row r="24" spans="1:18" s="4" customFormat="1">
+    <row r="24" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -987,7 +1009,7 @@
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
     </row>
-    <row r="25" spans="1:18" s="4" customFormat="1">
+    <row r="25" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1007,7 +1029,7 @@
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
     </row>
-    <row r="26" spans="1:18" s="4" customFormat="1">
+    <row r="26" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1027,7 +1049,7 @@
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
     </row>
-    <row r="27" spans="1:18" s="4" customFormat="1">
+    <row r="27" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1047,7 +1069,7 @@
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
     </row>
-    <row r="28" spans="1:18" s="4" customFormat="1">
+    <row r="28" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1067,7 +1089,7 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
     </row>
-    <row r="29" spans="1:18" s="4" customFormat="1" ht="15.75" thickBot="1">
+    <row r="29" spans="1:18" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1087,26 +1109,26 @@
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="21" t="s">
+      <c r="C30" s="20"/>
+      <c r="D30" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="21" t="s">
+      <c r="E30" s="20"/>
+      <c r="F30" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="22"/>
-      <c r="H30" s="21" t="s">
+      <c r="G30" s="20"/>
+      <c r="H30" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I30" s="22"/>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="I30" s="20"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
@@ -1123,7 +1145,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
@@ -1140,7 +1162,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1179,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
@@ -1174,7 +1196,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1185,7 +1207,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1196,7 +1218,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1207,7 +1229,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1218,7 +1240,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1229,7 +1251,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1240,7 +1262,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1251,7 +1273,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1262,7 +1284,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:18" ht="15.75" thickBot="1">
+    <row r="43" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1273,24 +1295,24 @@
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:18" s="4" customFormat="1">
-      <c r="A44" s="6"/>
-      <c r="B44" s="19" t="s">
+    <row r="44" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="19" t="s">
+      <c r="C44" s="18"/>
+      <c r="D44" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="19" t="s">
+      <c r="E44" s="18"/>
+      <c r="F44" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G44" s="20"/>
-      <c r="H44" s="19" t="s">
+      <c r="G44" s="18"/>
+      <c r="H44" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I44" s="20"/>
+      <c r="I44" s="18"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
@@ -1301,10 +1323,16 @@
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
     </row>
-    <row r="45" spans="1:18" s="4" customFormat="1">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+    <row r="45" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="1">
+        <v>10</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1">
@@ -1323,10 +1351,16 @@
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
     </row>
-    <row r="46" spans="1:18" s="4" customFormat="1">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+    <row r="46" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="1">
+        <v>10</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1">
@@ -1345,10 +1379,16 @@
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
     </row>
-    <row r="47" spans="1:18" s="4" customFormat="1">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+    <row r="47" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1">
@@ -1367,10 +1407,16 @@
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
     </row>
-    <row r="48" spans="1:18" s="4" customFormat="1">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+    <row r="48" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="1">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1">
@@ -1389,7 +1435,7 @@
       <c r="Q48" s="5"/>
       <c r="R48" s="5"/>
     </row>
-    <row r="49" spans="1:18" s="4" customFormat="1">
+    <row r="49" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1409,7 +1455,7 @@
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
     </row>
-    <row r="50" spans="1:18" s="4" customFormat="1">
+    <row r="50" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1429,7 +1475,7 @@
       <c r="Q50" s="5"/>
       <c r="R50" s="5"/>
     </row>
-    <row r="51" spans="1:18" s="4" customFormat="1">
+    <row r="51" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1449,7 +1495,7 @@
       <c r="Q51" s="5"/>
       <c r="R51" s="5"/>
     </row>
-    <row r="52" spans="1:18" s="4" customFormat="1">
+    <row r="52" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1469,7 +1515,7 @@
       <c r="Q52" s="5"/>
       <c r="R52" s="5"/>
     </row>
-    <row r="53" spans="1:18" s="4" customFormat="1">
+    <row r="53" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1489,7 +1535,7 @@
       <c r="Q53" s="5"/>
       <c r="R53" s="5"/>
     </row>
-    <row r="54" spans="1:18" s="4" customFormat="1">
+    <row r="54" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1509,7 +1555,7 @@
       <c r="Q54" s="5"/>
       <c r="R54" s="5"/>
     </row>
-    <row r="55" spans="1:18" s="4" customFormat="1">
+    <row r="55" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1529,7 +1575,7 @@
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
     </row>
-    <row r="56" spans="1:18" s="4" customFormat="1" ht="15.75" thickBot="1">
+    <row r="56" spans="1:18" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -1551,6 +1597,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="F44:G44"/>
@@ -1563,14 +1617,6 @@
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="H30:I30"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1578,24 +1624,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>